<commit_message>
Change the UI's position in App Designer
</commit_message>
<xml_diff>
--- a/UI_Testing/UI_Development/Attempt2/results_extra.xlsx
+++ b/UI_Testing/UI_Development/Attempt2/results_extra.xlsx
@@ -13,7 +13,391 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2310" uniqueCount="1344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2530" uniqueCount="1472">
+  <si>
+    <t>final_1</t>
+  </si>
+  <si>
+    <t>final_2</t>
+  </si>
+  <si>
+    <t>final_3</t>
+  </si>
+  <si>
+    <t>final_4</t>
+  </si>
+  <si>
+    <t>final_5</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Contrast</t>
+  </si>
+  <si>
+    <t>Correlation</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Homogeneity</t>
+  </si>
+  <si>
+    <t>Actual Condition</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>final_1</t>
+  </si>
+  <si>
+    <t>final_2</t>
+  </si>
+  <si>
+    <t>final_3</t>
+  </si>
+  <si>
+    <t>final_4</t>
+  </si>
+  <si>
+    <t>final_5</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Contrast</t>
+  </si>
+  <si>
+    <t>Correlation</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>Homogeneity</t>
+  </si>
+  <si>
+    <t>Actual Condition</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
   <si>
     <t>final_1</t>
   </si>
@@ -4065,7 +4449,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -4115,11 +4499,15 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -4163,6 +4551,10 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="43" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="44" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4184,865 +4576,869 @@
   <sheetData>
     <row r="3">
       <c r="B3" s="0" t="s">
-        <v>1312</v>
+        <v>1440</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>1313</v>
+        <v>1441</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>1314</v>
+        <v>1442</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>1315</v>
+        <v>1443</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>1316</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="0">
-        <v>0.0043305058913799812</v>
+        <v>0.0021786305014003435</v>
       </c>
       <c r="C4" s="0">
-        <v>0.97058615281257665</v>
+        <v>0.9896198038413121</v>
       </c>
       <c r="D4" s="0">
-        <v>0.84846147138245076</v>
+        <v>0.78794275071223474</v>
       </c>
       <c r="E4" s="0">
-        <v>0.99783474705430986</v>
+        <v>0.99891068474929967</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>1317</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="0">
-        <v>0.0035823183112938103</v>
+        <v>0.0022311851845481586</v>
       </c>
       <c r="C5" s="0">
-        <v>0.97331719366984626</v>
+        <v>0.98650445735398462</v>
       </c>
       <c r="D5" s="0">
-        <v>0.86217483457586019</v>
+        <v>0.83244622944556768</v>
       </c>
       <c r="E5" s="0">
-        <v>0.99820884084435313</v>
+        <v>0.99888440740772599</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>1317</v>
+        <v>1445</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="0">
-        <v>0.0070566606372111998</v>
+        <v>0.0025818682520981264</v>
       </c>
       <c r="C6" s="0">
-        <v>0.95632765129983521</v>
+        <v>0.98854737321217423</v>
       </c>
       <c r="D6" s="0">
-        <v>0.83141124597098415</v>
+        <v>0.77198583955688438</v>
       </c>
       <c r="E6" s="0">
-        <v>0.99647166968139433</v>
+        <v>0.99870906587395092</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>1318</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="0">
-        <v>0.0077112053273248994</v>
+        <v>0.0051847583774553788</v>
       </c>
       <c r="C7" s="0">
-        <v>0.96323916929432551</v>
+        <v>0.98960538826973954</v>
       </c>
       <c r="D7" s="0">
-        <v>0.78258136201820183</v>
+        <v>0.49604923795102202</v>
       </c>
       <c r="E7" s="0">
-        <v>0.99614439733633753</v>
+        <v>0.99740762081127232</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>1318</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" s="0">
-        <v>0.00062683403899939708</v>
+        <v>0.003214435529259103</v>
       </c>
       <c r="C8" s="0">
-        <v>0.92322841645578568</v>
+        <v>0.99357002138898376</v>
       </c>
       <c r="D8" s="0">
-        <v>0.99120863626261591</v>
+        <v>0.49688202118643354</v>
       </c>
       <c r="E8" s="0">
-        <v>0.99968658298050017</v>
+        <v>0.99839278223537042</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>1319</v>
+        <v>1447</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" s="0">
-        <v>0.0058249699721651289</v>
+        <v>0.0031198370995930355</v>
       </c>
       <c r="C9" s="0">
-        <v>0.90797031056376221</v>
+        <v>0.99374838575493196</v>
       </c>
       <c r="D9" s="0">
-        <v>0.9309144951380397</v>
+        <v>0.49784485330895134</v>
       </c>
       <c r="E9" s="0">
-        <v>0.99708751501391757</v>
+        <v>0.99844008145020346</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>1320</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" s="0">
-        <v>0.010788998680399684</v>
+        <v>0.0035288080884523982</v>
       </c>
       <c r="C10" s="0">
-        <v>0.94847854384152885</v>
+        <v>0.99289088289635763</v>
       </c>
       <c r="D10" s="0">
-        <v>0.77991952824248822</v>
+        <v>0.50010581899350126</v>
       </c>
       <c r="E10" s="0">
-        <v>0.99460550065980002</v>
+        <v>0.99823559595577382</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>1320</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="0">
-        <v>0.012886408307844313</v>
+        <v>0.0037925370438850717</v>
       </c>
       <c r="C11" s="0">
-        <v>0.94210273716929671</v>
+        <v>0.99239972028556156</v>
       </c>
       <c r="D11" s="0">
-        <v>0.76470594603409314</v>
+        <v>0.4972221796520998</v>
       </c>
       <c r="E11" s="0">
-        <v>0.99355679584607792</v>
+        <v>0.99810373147805753</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>1320</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" s="0">
-        <v>0.011477942799482862</v>
+        <v>0.0027165993488952526</v>
       </c>
       <c r="C12" s="0">
-        <v>0.95020130521611723</v>
+        <v>0.99279807124818298</v>
       </c>
       <c r="D12" s="0">
-        <v>0.7581669803996367</v>
+        <v>0.62008636178712873</v>
       </c>
       <c r="E12" s="0">
-        <v>0.99426102860025845</v>
+        <v>0.99864170032555244</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>1320</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" s="0">
-        <v>0.0045311692270352758</v>
+        <v>0.0025990679665828659</v>
       </c>
       <c r="C13" s="0">
-        <v>0.98146908869194682</v>
+        <v>0.9914208452660892</v>
       </c>
       <c r="D13" s="0">
-        <v>0.75096985905960423</v>
+        <v>0.69445616723091042</v>
       </c>
       <c r="E13" s="0">
-        <v>0.99773441538648222</v>
+        <v>0.9987004660167087</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>1321</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" s="0">
-        <v>0.0048273865320502349</v>
+        <v>0.0025570242200646134</v>
       </c>
       <c r="C14" s="0">
-        <v>0.98370859287657608</v>
+        <v>0.99270427298617803</v>
       </c>
       <c r="D14" s="0">
-        <v>0.69888102575816557</v>
+        <v>0.64696707213978832</v>
       </c>
       <c r="E14" s="0">
-        <v>0.99758630673397475</v>
+        <v>0.99872148788996762</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>1322</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" s="0">
-        <v>0.010702044568282389</v>
+        <v>0.0032096578307911198</v>
       </c>
       <c r="C15" s="0">
-        <v>0.94416163197763725</v>
+        <v>0.99133831984190346</v>
       </c>
       <c r="D15" s="0">
-        <v>0.79775136177281991</v>
+        <v>0.62624230294165883</v>
       </c>
       <c r="E15" s="0">
-        <v>0.99464897771585892</v>
+        <v>0.99839517108460452</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>1323</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" s="0">
-        <v>0.0059186128621375993</v>
+        <v>0.0025866459505661096</v>
       </c>
       <c r="C16" s="0">
-        <v>0.98258193315077647</v>
+        <v>0.99312954556652455</v>
       </c>
       <c r="D16" s="0">
-        <v>0.65431907259035682</v>
+        <v>0.62093170975561784</v>
       </c>
       <c r="E16" s="0">
-        <v>0.99704069356893121</v>
+        <v>0.99870667702471683</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>1323</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" s="0">
-        <v>0.004257884874666636</v>
+        <v>0.0024863142827384623</v>
       </c>
       <c r="C17" s="0">
-        <v>0.98827356423118484</v>
+        <v>0.99337485220897348</v>
       </c>
       <c r="D17" s="0">
-        <v>0.63265887626159634</v>
+        <v>0.6222355174262979</v>
       </c>
       <c r="E17" s="0">
-        <v>0.99787105756266681</v>
+        <v>0.99875684285863064</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>1324</v>
+        <v>1452</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" s="0">
-        <v>0.0077838263440382447</v>
+        <v>0.004525435988873696</v>
       </c>
       <c r="C18" s="0">
-        <v>0.97134155129533339</v>
+        <v>0.99056991355941848</v>
       </c>
       <c r="D18" s="0">
-        <v>0.72067007332427313</v>
+        <v>0.51560167066457474</v>
       </c>
       <c r="E18" s="0">
-        <v>0.99610808682798102</v>
+        <v>0.997737282005563</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>1325</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" s="0">
-        <v>0.0058154145752291626</v>
+        <v>0.0055191972702142034</v>
       </c>
       <c r="C19" s="0">
-        <v>0.96610384167052643</v>
+        <v>0.9791855543276291</v>
       </c>
       <c r="D19" s="0">
-        <v>0.82265280937649032</v>
+        <v>0.72934939750090655</v>
       </c>
       <c r="E19" s="0">
-        <v>0.99709229271238553</v>
+        <v>0.99724040136489278</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>1326</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" s="0">
-        <v>0.0036874276775894408</v>
+        <v>0.0019005684505637207</v>
       </c>
       <c r="C20" s="0">
-        <v>0.97758081914203265</v>
+        <v>0.99074523767648925</v>
       </c>
       <c r="D20" s="0">
-        <v>0.83184970168536321</v>
+        <v>0.7927419135017485</v>
       </c>
       <c r="E20" s="0">
-        <v>0.99815628616120533</v>
+        <v>0.99904971577471802</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>1327</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" s="0">
-        <v>0.0026888886977809502</v>
+        <v>0.0024394928377522267</v>
       </c>
       <c r="C21" s="0">
-        <v>0.98317313890742608</v>
+        <v>0.99458577639148715</v>
       </c>
       <c r="D21" s="0">
-        <v>0.83752093874877975</v>
+        <v>0.54699533043154625</v>
       </c>
       <c r="E21" s="0">
-        <v>0.99865555565110964</v>
+        <v>0.99878025358112388</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>1328</v>
+        <v>1456</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" s="0">
-        <v>0.0092467576149347034</v>
+        <v>0.0048684747388748903</v>
       </c>
       <c r="C22" s="0">
-        <v>0.97445361364154626</v>
+        <v>0.9883282068313306</v>
       </c>
       <c r="D22" s="0">
-        <v>0.62887922996523227</v>
+        <v>0.57804067870974551</v>
       </c>
       <c r="E22" s="0">
-        <v>0.99537662119253267</v>
+        <v>0.99756576263056251</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>1329</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" s="0">
-        <v>0.014939863109383495</v>
+        <v>0.0025780460933237399</v>
       </c>
       <c r="C23" s="0">
-        <v>0.95996008200223248</v>
+        <v>0.99425598900778334</v>
       </c>
       <c r="D23" s="0">
-        <v>0.6121591179587238</v>
+        <v>0.54860527854300234</v>
       </c>
       <c r="E23" s="0">
-        <v>0.99253006844530833</v>
+        <v>0.99871097695333799</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>1330</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" s="0">
-        <v>0.0069114186037845101</v>
+        <v>0.0026793333008449838</v>
       </c>
       <c r="C24" s="0">
-        <v>0.97631139961808744</v>
+        <v>0.99462189241698218</v>
       </c>
       <c r="D24" s="0">
-        <v>0.70137497475629829</v>
+        <v>0.49913526393747787</v>
       </c>
       <c r="E24" s="0">
-        <v>0.99654429069810779</v>
+        <v>0.9986603333495776</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>1331</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" s="0">
-        <v>0.0054064435863697994</v>
+        <v>0.0026678668245218242</v>
       </c>
       <c r="C25" s="0">
-        <v>0.97746964526311109</v>
+        <v>0.99140042713401932</v>
       </c>
       <c r="D25" s="0">
-        <v>0.7546601378982345</v>
+        <v>0.68710676983208174</v>
       </c>
       <c r="E25" s="0">
-        <v>0.99729677820681495</v>
+        <v>0.99866606658773904</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>1332</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" s="0">
-        <v>0.0045311692270352758</v>
+        <v>0.0024767588858024955</v>
       </c>
       <c r="C26" s="0">
-        <v>0.98872469756540537</v>
+        <v>0.99415992696350419</v>
       </c>
       <c r="D26" s="0">
-        <v>0.59362260496151142</v>
+        <v>0.57343213037586549</v>
       </c>
       <c r="E26" s="0">
-        <v>0.99773441538648222</v>
+        <v>0.99876162055709872</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>1333</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" s="0">
-        <v>0.0034428095160287005</v>
+        <v>0.0023515831859413357</v>
       </c>
       <c r="C27" s="0">
-        <v>0.98958302671868781</v>
+        <v>0.99369180460118178</v>
       </c>
       <c r="D27" s="0">
-        <v>0.66606905815162376</v>
+        <v>0.62487171075039838</v>
       </c>
       <c r="E27" s="0">
-        <v>0.99827859524198559</v>
+        <v>0.99882420840702935</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>1334</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" s="0">
-        <v>0.0020266996901184774</v>
+        <v>0.00308448213092996</v>
       </c>
       <c r="C28" s="0">
-        <v>0.93687785614741759</v>
+        <v>0.99323755616560749</v>
       </c>
       <c r="D28" s="0">
-        <v>0.9658698213800333</v>
+        <v>0.54080558655258204</v>
       </c>
       <c r="E28" s="0">
-        <v>0.99898665015494081</v>
+        <v>0.99845775893453514</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>1335</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" s="0">
-        <v>0</v>
-      </c>
-      <c r="C29" s="0"/>
+        <v>0.005512508492359027</v>
+      </c>
+      <c r="C29" s="0">
+        <v>0.98434328702826845</v>
+      </c>
       <c r="D29" s="0">
-        <v>1</v>
+        <v>0.64243193999861903</v>
       </c>
       <c r="E29" s="0">
-        <v>1</v>
+        <v>0.99724374575382047</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>1336</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" s="0">
-        <v>0</v>
-      </c>
-      <c r="C30" s="0"/>
+        <v>0.0034475872144966837</v>
+      </c>
+      <c r="C30" s="0">
+        <v>0.99182439593584315</v>
+      </c>
       <c r="D30" s="0">
-        <v>1</v>
+        <v>0.57487225149377041</v>
       </c>
       <c r="E30" s="0">
-        <v>1</v>
+        <v>0.99827620639275161</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>1336</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" s="0">
-        <v>0.0088731415947384158</v>
+        <v>0.0030128166539102118</v>
       </c>
       <c r="C31" s="0">
-        <v>0.97373642397886295</v>
+        <v>0.99130133849615998</v>
       </c>
       <c r="D31" s="0">
-        <v>0.65335587905055803</v>
+        <v>0.65064220897602298</v>
       </c>
       <c r="E31" s="0">
-        <v>0.99556342920263086</v>
+        <v>0.99849359167304486</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>1336</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" s="0">
-        <v>0.0074188101810843277</v>
+        <v>0.002726154745831219</v>
       </c>
       <c r="C32" s="0">
-        <v>0.97673230942209588</v>
+        <v>0.9920805027246874</v>
       </c>
       <c r="D32" s="0">
-        <v>0.67379022378933262</v>
+        <v>0.65304796904085205</v>
       </c>
       <c r="E32" s="0">
-        <v>0.99629059490945782</v>
+        <v>0.99863692262708437</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>1337</v>
+        <v>1465</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" s="0">
-        <v>0.0063791829944511809</v>
+        <v>0.0050720046936109748</v>
       </c>
       <c r="C33" s="0">
-        <v>0.97863950936873079</v>
+        <v>0.98509761689238107</v>
       </c>
       <c r="D33" s="0">
-        <v>0.69501748147036435</v>
+        <v>0.65460515635313588</v>
       </c>
       <c r="E33" s="0">
-        <v>0.99681040850277436</v>
+        <v>0.9974639976531946</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>1338</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" s="0">
-        <v>0.0074818758008617058</v>
+        <v>0.0046104790216037967</v>
       </c>
       <c r="C34" s="0">
-        <v>0.97811400833628581</v>
+        <v>0.98820018517256836</v>
       </c>
       <c r="D34" s="0">
-        <v>0.6507172694983232</v>
+        <v>0.60468608485972386</v>
       </c>
       <c r="E34" s="0">
-        <v>0.99625906209956927</v>
+        <v>0.99769476048919803</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>1339</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" s="0">
-        <v>0.0039024241086486854</v>
+        <v>0.0019550342130987292</v>
       </c>
       <c r="C35" s="0">
-        <v>0.97655102013103079</v>
+        <v>0.99044274964904722</v>
       </c>
       <c r="D35" s="0">
-        <v>0.82969089091157433</v>
+        <v>0.79348846554041019</v>
       </c>
       <c r="E35" s="0">
-        <v>0.99804878794567564</v>
+        <v>0.99902248289345064</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>1340</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" s="0">
-        <v>0.0038479583461136766</v>
+        <v>0.0031045484644954893</v>
       </c>
       <c r="C36" s="0">
-        <v>0.97856299982791939</v>
+        <v>0.9862223382158557</v>
       </c>
       <c r="D36" s="0">
-        <v>0.81666606403534736</v>
+        <v>0.77157306222292565</v>
       </c>
       <c r="E36" s="0">
-        <v>0.99807602082694302</v>
+        <v>0.99844772576775231</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>1340</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" s="0">
-        <v>0.0027223325870568325</v>
+        <v>0.0024710256476409157</v>
       </c>
       <c r="C37" s="0">
-        <v>0.973445132059366</v>
+        <v>0.99455097832992179</v>
       </c>
       <c r="D37" s="0">
-        <v>0.89476780773294018</v>
+        <v>0.54405447457945755</v>
       </c>
       <c r="E37" s="0">
-        <v>0.99863883370647155</v>
+        <v>0.99876448717617938</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>1340</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" s="0">
-        <v>0.0027672429526558748</v>
+        <v>0.0036769167409598778</v>
       </c>
       <c r="C38" s="0">
-        <v>0.96756783696313176</v>
+        <v>0.9913694604617499</v>
       </c>
       <c r="D38" s="0">
-        <v>0.91191638157493637</v>
+        <v>0.57030104347638078</v>
       </c>
       <c r="E38" s="0">
-        <v>0.99861637852367202</v>
+        <v>0.9981615416295202</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>1340</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" s="0">
-        <v>0.0039492455536349206</v>
+        <v>0.0044384818767564012</v>
       </c>
       <c r="C39" s="0">
-        <v>0.97461640138163153</v>
+        <v>0.9896212800548545</v>
       </c>
       <c r="D39" s="0">
-        <v>0.84048377922422479</v>
+        <v>0.56792907036750706</v>
       </c>
       <c r="E39" s="0">
-        <v>0.99802537722318241</v>
+        <v>0.99778075906162167</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>1340</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" s="0">
-        <v>0.0022130299303698225</v>
+        <v>0.0016377950348246441</v>
       </c>
       <c r="C40" s="0">
-        <v>0.98486735132050707</v>
+        <v>0.99143931378224959</v>
       </c>
       <c r="D40" s="0">
-        <v>0.85154979341466142</v>
+        <v>0.80704902863605887</v>
       </c>
       <c r="E40" s="0">
-        <v>0.99889348503481523</v>
+        <v>0.99918110248258774</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>1340</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" s="0">
-        <v>0.0039731340459748365</v>
+        <v>0.0039425567757797441</v>
       </c>
       <c r="C41" s="0">
-        <v>0.97611829625085489</v>
+        <v>0.98956792570473373</v>
       </c>
       <c r="D41" s="0">
-        <v>0.82967537378053413</v>
+        <v>0.61814653973565692</v>
       </c>
       <c r="E41" s="0">
-        <v>0.99801343297701262</v>
+        <v>0.99802872161211009</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>1340</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" s="0">
-        <v>0.0029315957799544972</v>
+        <v>0.0016416171935990306</v>
       </c>
       <c r="C42" s="0">
-        <v>0.9713383714946926</v>
+        <v>0.98575564603301224</v>
       </c>
       <c r="D42" s="0">
-        <v>0.89479405319698635</v>
+        <v>0.88311420885550629</v>
       </c>
       <c r="E42" s="0">
-        <v>0.99853420211002275</v>
+        <v>0.99917919140320055</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>1340</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" s="0">
-        <v>0.0044279709401268382</v>
+        <v>0.0023640052019580919</v>
       </c>
       <c r="C43" s="0">
-        <v>0.96282962700383012</v>
+        <v>0.9918225137888288</v>
       </c>
       <c r="D43" s="0">
-        <v>0.87646528391620049</v>
+        <v>0.70855455328138373</v>
       </c>
       <c r="E43" s="0">
-        <v>0.99778601452993654</v>
+        <v>0.998817997399021</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>1340</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" s="0">
-        <v>0.0096872614136827555</v>
+        <v>0.0024614702507049493</v>
       </c>
       <c r="C44" s="0">
-        <v>0.95836151380460111</v>
+        <v>0.99362832533223211</v>
       </c>
       <c r="D44" s="0">
-        <v>0.75775495811422977</v>
+        <v>0.61123009843123355</v>
       </c>
       <c r="E44" s="0">
-        <v>0.99515636929315865</v>
+        <v>0.99876926487464757</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>1341</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" s="0">
-        <v>0.0063065619777378365</v>
+        <v>0.002020010912263301</v>
       </c>
       <c r="C45" s="0">
-        <v>0.96260707994081862</v>
+        <v>0.99166814592097263</v>
       </c>
       <c r="D45" s="0">
-        <v>0.82507663169982015</v>
+        <v>0.75553972363910959</v>
       </c>
       <c r="E45" s="0">
-        <v>0.9968467190111312</v>
+        <v>0.9989899945438685</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>1341</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" s="0">
-        <v>0.0018986573711765274</v>
+        <v>0.0025742239345493533</v>
       </c>
       <c r="C46" s="0">
-        <v>0.91647844513213106</v>
+        <v>0.99467223861739806</v>
       </c>
       <c r="D46" s="0">
-        <v>0.97537240412495851</v>
+        <v>0.51426062571578579</v>
       </c>
       <c r="E46" s="0">
-        <v>0.99905067131441172</v>
+        <v>0.99871288803272529</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>1341</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" s="0">
-        <v>0.0067699987291322079</v>
+        <v>0.0022827843280023774</v>
       </c>
       <c r="C47" s="0">
-        <v>0.96194030056039903</v>
+        <v>0.99227886168012958</v>
       </c>
       <c r="D47" s="0">
-        <v>0.8153974265777969</v>
+        <v>0.70206856934861162</v>
       </c>
       <c r="E47" s="0">
-        <v>0.99661500063543385</v>
+        <v>0.99885860783599878</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>1342</v>
+        <v>1470</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" s="0">
-        <v>0.0065378025835882234</v>
+        <v>0.0033883437534936922</v>
       </c>
       <c r="C48" s="0">
-        <v>0.96913032739399041</v>
+        <v>0.98678689817872267</v>
       </c>
       <c r="D48" s="0">
-        <v>0.78171770602390012</v>
+        <v>0.7401849593683727</v>
       </c>
       <c r="E48" s="0">
-        <v>0.99673109870820586</v>
+        <v>0.99830582812325319</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>1343</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="49">
       <c r="B49" s="0">
-        <v>0.0079233351393033537</v>
+        <v>0.0065894017270424418</v>
       </c>
       <c r="C49" s="0">
-        <v>0.95932582973447522</v>
+        <v>0.96628510778972188</v>
       </c>
       <c r="D49" s="0">
-        <v>0.79733927761690493</v>
+        <v>0.79800917809100125</v>
       </c>
       <c r="E49" s="0">
-        <v>0.99603833243034834</v>
+        <v>0.99670529913647865</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>1343</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="50">
       <c r="B50" s="0">
-        <v>0.0063581611211920549</v>
+        <v>0.002030521848892864</v>
       </c>
       <c r="C50" s="0">
-        <v>0.9458995492162916</v>
+        <v>0.99395985466012415</v>
       </c>
       <c r="D50" s="0">
-        <v>0.87615716078869899</v>
+        <v>0.66180257636249462</v>
       </c>
       <c r="E50" s="0">
-        <v>0.99682091943940399</v>
+        <v>0.99898473907555352</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>1343</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="51">
       <c r="B51" s="0">
-        <v>0.0067002443314996525</v>
+        <v>0.0029851060027959093</v>
       </c>
       <c r="C51" s="0">
-        <v>0.96178078712484172</v>
+        <v>0.99028370181840097</v>
       </c>
       <c r="D51" s="0">
-        <v>0.81803375613625962</v>
+        <v>0.68979712788366254</v>
       </c>
       <c r="E51" s="0">
-        <v>0.9966498778342503</v>
+        <v>0.99850744699860217</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>1343</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="52">
       <c r="B52" s="0">
-        <v>0.004932495898345865</v>
+        <v>0.0023257836142142265</v>
       </c>
       <c r="C52" s="0">
-        <v>0.97330585968277328</v>
+        <v>0.99011240125617828</v>
       </c>
       <c r="D52" s="0">
-        <v>0.81031360739515845</v>
+        <v>0.76245733615164402</v>
       </c>
       <c r="E52" s="0">
-        <v>0.99753375205082695</v>
+        <v>0.99883710819289295</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>1343</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="53">
       <c r="B53" s="0">
-        <v>0.010096232402542118</v>
+        <v>0.0059425013544775153</v>
       </c>
       <c r="C53" s="0">
-        <v>0.96229624573572881</v>
+        <v>0.97371037485414313</v>
       </c>
       <c r="D53" s="0">
-        <v>0.72222779451644059</v>
+        <v>0.76805302168907841</v>
       </c>
       <c r="E53" s="0">
-        <v>0.9949518837987289</v>
+        <v>0.9970287493227612</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>1343</v>
+        <v>1471</v>
       </c>
     </row>
   </sheetData>

</xml_diff>